<commit_message>
db uploader 1차 완료
</commit_message>
<xml_diff>
--- a/user.xlsx
+++ b/user.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saint\OneDrive\dev\backend\go\dbUploader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87206C4-4E86-4F99-AD90-F7943FD53B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89AF8B0-8AF8-4723-967C-92DA0B331652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40440" yWindow="7815" windowWidth="17280" windowHeight="9090" xr2:uid="{969E9B9B-3E3B-4BC3-BEBF-AF4520235F12}"/>
+    <workbookView xWindow="38280" yWindow="5100" windowWidth="23280" windowHeight="12600" xr2:uid="{969E9B9B-3E3B-4BC3-BEBF-AF4520235F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,11 +108,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>smallint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SERIAL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F15984-E632-4B72-939C-054BE26B8D60}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -516,7 +516,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -571,7 +571,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -587,7 +587,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>